<commit_message>
'Enter Share Skill; test added
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\recreateMF\MarsFramework\MarsFramework\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\onboarding.nunit\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
-    <sheet name="SignUp" sheetId="3" r:id="rId1"/>
-    <sheet name="SignIn" sheetId="1" r:id="rId2"/>
-    <sheet name="Profile" sheetId="2" r:id="rId3"/>
+    <sheet name="ShareSkill" sheetId="4" r:id="rId1"/>
+    <sheet name="SignUp" sheetId="3" r:id="rId2"/>
+    <sheet name="SignIn" sheetId="1" r:id="rId3"/>
+    <sheet name="Profile" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Url</t>
   </si>
@@ -35,15 +36,9 @@
     <t>Language</t>
   </si>
   <si>
-    <t>English</t>
-  </si>
-  <si>
     <t>Skill</t>
   </si>
   <si>
-    <t>Automation Testing</t>
-  </si>
-  <si>
     <t>University</t>
   </si>
   <si>
@@ -53,24 +48,15 @@
     <t>Certificate</t>
   </si>
   <si>
-    <t>ISTQB</t>
-  </si>
-  <si>
     <t>CertifiedFrom</t>
   </si>
   <si>
-    <t>ANZTB</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>AvailableTime</t>
   </si>
   <si>
-    <t>Full time</t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
@@ -89,33 +75,6 @@
     <t>ConfirmPswd</t>
   </si>
   <si>
-    <t>Venugan</t>
-  </si>
-  <si>
-    <t>Vidhya</t>
-  </si>
-  <si>
-    <t>vidhyav9@gmail.com</t>
-  </si>
-  <si>
-    <t>Ithika2015</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>Melbourne</t>
-  </si>
-  <si>
-    <t>Amrita School Of Engineering</t>
-  </si>
-  <si>
-    <t>B.Tech</t>
-  </si>
-  <si>
-    <t>3 years as Oracle Developer and 2 years as Project Management Operations Lead</t>
-  </si>
-  <si>
     <t>anton.regis@gmail.com</t>
   </si>
   <si>
@@ -123,13 +82,103 @@
   </si>
   <si>
     <t>http://localhost:5000</t>
+  </si>
+  <si>
+    <t>Anton</t>
+  </si>
+  <si>
+    <t>Regis</t>
+  </si>
+  <si>
+    <t>triboyph@yahoo.com</t>
+  </si>
+  <si>
+    <t>industryconnect2022</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Service Type</t>
+  </si>
+  <si>
+    <t>Location Type</t>
+  </si>
+  <si>
+    <t>Available days</t>
+  </si>
+  <si>
+    <t>Skill Trade</t>
+  </si>
+  <si>
+    <t>Skill-Exchange</t>
+  </si>
+  <si>
+    <t>Work Samples</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Subcategory</t>
+  </si>
+  <si>
+    <t>Programming &amp; Tech</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Hourly basis service</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Start date</t>
+  </si>
+  <si>
+    <t>End date</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>randomfile.txt</t>
+  </si>
+  <si>
+    <t>Software Testing</t>
+  </si>
+  <si>
+    <t>MWF, 8am-3pm</t>
+  </si>
+  <si>
+    <t>Start time</t>
+  </si>
+  <si>
+    <t>End time</t>
+  </si>
+  <si>
+    <t>Develop test automation scripts with a specialization in C Sharp, Selenium and other tools.</t>
+  </si>
+  <si>
+    <t>10/05/2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,26 +186,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -174,21 +210,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -491,68 +524,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="12" width="15.42578125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" customWidth="1"/>
+    <col min="15" max="15" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="3">
+        <v>44773</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="L2" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="M2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2">
+        <v>30</v>
+      </c>
+      <c r="O2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -564,25 +723,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -591,12 +750,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,68 +770,36 @@
     <col min="10" max="10" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EditShareSkill() and DeleteShareSkill() added.
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Url</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Location Type</t>
   </si>
   <si>
-    <t>Available days</t>
-  </si>
-  <si>
     <t>Skill Trade</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>Software Testing</t>
   </si>
   <si>
-    <t>MWF, 8am-3pm</t>
-  </si>
-  <si>
     <t>Start time</t>
   </si>
   <si>
@@ -172,6 +166,24 @@
   </si>
   <si>
     <t>10/05/2022</t>
+  </si>
+  <si>
+    <t>Quality Assurance</t>
+  </si>
+  <si>
+    <t>Code test automation scripts with a specialization in C Sharp, Selenium and other tools.</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>One-off service</t>
+  </si>
+  <si>
+    <t>Skill-exchanges</t>
   </si>
 </sst>
 </file>
@@ -213,13 +225,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,28 +552,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="10" width="15.42578125" customWidth="1"/>
-    <col min="11" max="12" width="15.42578125" style="5" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" customWidth="1"/>
-    <col min="15" max="15" width="52.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -556,7 +587,7 @@
         <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>26</v>
@@ -568,19 +599,19 @@
         <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>30</v>
@@ -591,59 +622,86 @@
       <c r="O1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="2" spans="1:15" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="6">
+        <v>44773</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0.625</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="4">
+        <v>30</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="3">
-        <v>44773</v>
-      </c>
-      <c r="J2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="L2" s="5">
-        <v>0.625</v>
-      </c>
-      <c r="M2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2">
-        <v>30</v>
-      </c>
-      <c r="O2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P2" t="s">
-        <v>33</v>
-      </c>
+      <c r="C3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="8">
+        <v>10</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+    </row>
+    <row r="5" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added 3x [TestCase] for EnterShareSkill and some code cleanup and improvements.
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ShareSkill" sheetId="4" r:id="rId1"/>
-    <sheet name="SignUp" sheetId="3" r:id="rId2"/>
-    <sheet name="SignIn" sheetId="1" r:id="rId3"/>
-    <sheet name="Profile" sheetId="2" r:id="rId4"/>
+    <sheet name="SSkillEdit" sheetId="5" r:id="rId2"/>
+    <sheet name="SignUp" sheetId="3" r:id="rId3"/>
+    <sheet name="SignIn" sheetId="1" r:id="rId4"/>
+    <sheet name="Profile" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
   <si>
     <t>Url</t>
   </si>
@@ -147,9 +148,6 @@
     <t>End date</t>
   </si>
   <si>
-    <t>Credit</t>
-  </si>
-  <si>
     <t>randomfile.txt</t>
   </si>
   <si>
@@ -165,35 +163,66 @@
     <t>Develop test automation scripts with a specialization in C Sharp, Selenium and other tools.</t>
   </si>
   <si>
-    <t>10/05/2022</t>
-  </si>
-  <si>
     <t>Quality Assurance</t>
   </si>
   <si>
-    <t>Code test automation scripts with a specialization in C Sharp, Selenium and other tools.</t>
-  </si>
-  <si>
     <t>Business</t>
   </si>
   <si>
-    <t>Hidden</t>
-  </si>
-  <si>
-    <t>One-off service</t>
-  </si>
-  <si>
     <t>Skill-exchanges</t>
+  </si>
+  <si>
+    <t>3D Animator</t>
+  </si>
+  <si>
+    <t>Video editing and 3D animation.</t>
+  </si>
+  <si>
+    <t>Video &amp; Animation</t>
+  </si>
+  <si>
+    <t>Promotional Videos</t>
+  </si>
+  <si>
+    <t>3D Studiomax</t>
+  </si>
+  <si>
+    <t>Design and create media advertisements.</t>
+  </si>
+  <si>
+    <t>Copy Writer</t>
+  </si>
+  <si>
+    <t>Writing &amp; Translation</t>
+  </si>
+  <si>
+    <t>Creative Writing</t>
+  </si>
+  <si>
+    <t>MS Word</t>
+  </si>
+  <si>
+    <t>31/09/2022</t>
+  </si>
+  <si>
+    <t>Testing 123... for deletion anyway.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -225,15 +254,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="18" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -245,7 +271,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -552,18 +587,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -573,7 +608,7 @@
     <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -605,10 +640,10 @@
         <v>40</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>29</v>
@@ -625,10 +660,10 @@
     </row>
     <row r="2" spans="1:15" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>34</v>
@@ -645,63 +680,124 @@
       <c r="G2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="6">
+      <c r="H2" s="8">
+        <v>44691</v>
+      </c>
+      <c r="I2" s="5">
         <v>44773</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="6">
         <v>0.29166666666666669</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="6">
         <v>0.625</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M2" s="4">
         <v>30</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:15" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="8">
+        <v>44743</v>
+      </c>
+      <c r="I3" s="5">
+        <v>44804</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="8" t="s">
+      <c r="M3" s="4">
+        <v>25</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="8">
-        <v>10</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>51</v>
+      <c r="O3" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
+    <row r="4" spans="1:15" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="8">
+        <v>44774</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="4">
+        <v>20</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -711,10 +807,101 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E19" sqref="A13:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,7 +952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -808,7 +995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added negative test cases
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
   <si>
     <t>Url</t>
   </si>
@@ -215,6 +215,24 @@
   </si>
   <si>
     <t>wsample2.png</t>
+  </si>
+  <si>
+    <t>fileupload_x64.exe</t>
+  </si>
+  <si>
+    <t>Missing title</t>
+  </si>
+  <si>
+    <t>Unslected Subcategory</t>
+  </si>
+  <si>
+    <t>Invalid file type upload</t>
+  </si>
+  <si>
+    <t>wsample4.png</t>
+  </si>
+  <si>
+    <t>wsample5.png</t>
   </si>
 </sst>
 </file>
@@ -596,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +708,7 @@
         <v>38</v>
       </c>
       <c r="H2" s="8">
-        <v>44691</v>
+        <v>44722</v>
       </c>
       <c r="I2" s="5">
         <v>44773</v>
@@ -805,6 +823,143 @@
         <v>61</v>
       </c>
       <c r="O4" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="8">
+        <v>44805</v>
+      </c>
+      <c r="I5" s="5">
+        <v>44865</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="4">
+        <v>20</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="8">
+        <v>44806</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="4">
+        <v>20</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="8">
+        <v>44869</v>
+      </c>
+      <c r="I7" s="5">
+        <v>44926</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.3125</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0.6875</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M7" s="4">
+        <v>20</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="O7" s="4" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>